<commit_message>
add file that parse data and create OLS and ridge model for it with all related output
</commit_message>
<xml_diff>
--- a/Model_rez_15/Hist_IR_Ridge_15.xlsx
+++ b/Model_rez_15/Hist_IR_Ridge_15.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>PredictReturn</t>
   </si>
@@ -28,160 +28,112 @@
     <t>Date</t>
   </si>
   <si>
-    <t>126.322271014</t>
-  </si>
-  <si>
-    <t>130.309592946</t>
-  </si>
-  <si>
-    <t>579.353471803</t>
-  </si>
-  <si>
-    <t>80.0386823996</t>
-  </si>
-  <si>
-    <t>160.457917679</t>
-  </si>
-  <si>
-    <t>74.0911024093</t>
-  </si>
-  <si>
-    <t>596.953011329</t>
-  </si>
-  <si>
-    <t>99.6734955913</t>
-  </si>
-  <si>
-    <t>82.7033298149</t>
-  </si>
-  <si>
-    <t>97.0415557953</t>
-  </si>
-  <si>
-    <t>551.662935179</t>
-  </si>
-  <si>
-    <t>99.5536634491</t>
-  </si>
-  <si>
-    <t>103.573694128</t>
+    <t>103.576550479</t>
+  </si>
+  <si>
+    <t>114.386943169</t>
+  </si>
+  <si>
+    <t>660.939436782</t>
+  </si>
+  <si>
+    <t>165.297124045</t>
+  </si>
+  <si>
+    <t>107.628741516</t>
+  </si>
+  <si>
+    <t>141.913225884</t>
+  </si>
+  <si>
+    <t>134.143912785</t>
+  </si>
+  <si>
+    <t>773.556073176</t>
+  </si>
+  <si>
+    <t>128.889487062</t>
+  </si>
+  <si>
+    <t>117.8267391</t>
+  </si>
+  <si>
+    <t>131.2105986</t>
+  </si>
+  <si>
+    <t>661.5823023</t>
+  </si>
+  <si>
+    <t>154.00336752</t>
+  </si>
+  <si>
+    <t>133.8033366</t>
+  </si>
+  <si>
+    <t>169.4276946</t>
   </si>
   <si>
     <t>164.27375532</t>
   </si>
   <si>
-    <t>169.4276946</t>
-  </si>
-  <si>
-    <t>555.847857</t>
-  </si>
-  <si>
-    <t>155.0271816</t>
-  </si>
-  <si>
-    <t>125.9233218</t>
-  </si>
-  <si>
-    <t>129.1651659</t>
-  </si>
-  <si>
-    <t>548.7253047</t>
-  </si>
-  <si>
-    <t>173.345508</t>
-  </si>
-  <si>
-    <t>131.2105986</t>
-  </si>
-  <si>
-    <t>137.8911411</t>
-  </si>
-  <si>
-    <t>514.0387161</t>
-  </si>
-  <si>
-    <t>133.8033366</t>
-  </si>
-  <si>
-    <t>117.8267391</t>
-  </si>
-  <si>
-    <t>37.9514843058</t>
-  </si>
-  <si>
-    <t>39.1181016543</t>
-  </si>
-  <si>
-    <t>-23.5056148032</t>
-  </si>
-  <si>
-    <t>74.9884992004</t>
-  </si>
-  <si>
-    <t>-34.5345958788</t>
-  </si>
-  <si>
-    <t>55.0740634907</t>
-  </si>
-  <si>
-    <t>-48.2277066293</t>
-  </si>
-  <si>
-    <t>73.6720124087</t>
-  </si>
-  <si>
-    <t>48.5072687851</t>
-  </si>
-  <si>
-    <t>40.8495853047</t>
-  </si>
-  <si>
-    <t>-37.6242190789</t>
-  </si>
-  <si>
-    <t>34.2496731509</t>
-  </si>
-  <si>
-    <t>14.2530449723</t>
+    <t>754.1580222</t>
+  </si>
+  <si>
+    <t>127.0782297</t>
+  </si>
+  <si>
+    <t>14.2501886208</t>
+  </si>
+  <si>
+    <t>16.8236554312</t>
+  </si>
+  <si>
+    <t>0.642865517731</t>
+  </si>
+  <si>
+    <t>-11.2937565245</t>
+  </si>
+  <si>
+    <t>26.1745950843</t>
+  </si>
+  <si>
+    <t>27.5144687164</t>
+  </si>
+  <si>
+    <t>30.1298425352</t>
+  </si>
+  <si>
+    <t>-19.3980509764</t>
+  </si>
+  <si>
+    <t>-1.8112573621</t>
+  </si>
+  <si>
+    <t>2017-05-05</t>
+  </si>
+  <si>
+    <t>2017-05-18</t>
+  </si>
+  <si>
+    <t>2017-04-10</t>
+  </si>
+  <si>
+    <t>2017-05-25</t>
+  </si>
+  <si>
+    <t>2017-05-08</t>
+  </si>
+  <si>
+    <t>2017-05-06</t>
   </si>
   <si>
     <t>2017-05-10</t>
   </si>
   <si>
-    <t>2017-05-06</t>
-  </si>
-  <si>
-    <t>2017-04-14</t>
-  </si>
-  <si>
-    <t>2017-05-23</t>
-  </si>
-  <si>
-    <t>2017-05-29</t>
-  </si>
-  <si>
-    <t>2017-05-19</t>
-  </si>
-  <si>
-    <t>2017-04-16</t>
-  </si>
-  <si>
-    <t>2017-05-20</t>
-  </si>
-  <si>
-    <t>2017-05-18</t>
-  </si>
-  <si>
-    <t>2017-05-09</t>
-  </si>
-  <si>
-    <t>2017-04-18</t>
-  </si>
-  <si>
-    <t>2017-05-08</t>
-  </si>
-  <si>
-    <t>2017-05-05</t>
+    <t>2017-04-11</t>
+  </si>
+  <si>
+    <t>2017-05-24</t>
   </si>
 </sst>
 </file>
@@ -539,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -567,13 +519,13 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -584,13 +536,13 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -601,13 +553,13 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -618,13 +570,13 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -635,13 +587,13 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -652,13 +604,13 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -669,13 +621,13 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -686,13 +638,13 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="E9" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -703,81 +655,13 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="E10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" t="s">
         <v>39</v>
-      </c>
-      <c r="E11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="1">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>